<commit_message>
creating a Tvec Func that uses fermentation_day
</commit_message>
<xml_diff>
--- a/data/ccb_ale1_tidy_fermdata.xlsx
+++ b/data/ccb_ale1_tidy_fermdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bertille/brewnalysis/brewnalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F979A617-808D-472F-AD56-CD100599E685}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45A3767-1B25-C846-8C19-17E256D984EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11805" yWindow="1485" windowWidth="11085" windowHeight="8400" xr2:uid="{9D76D547-5019-4ACE-9DBC-0E5075E032EF}"/>
+    <workbookView xWindow="11880" yWindow="700" windowWidth="19300" windowHeight="12580" xr2:uid="{9D76D547-5019-4ACE-9DBC-0E5075E032EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
@@ -125,7 +125,7 @@
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -189,15 +189,15 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -519,24 +519,24 @@
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="L394" sqref="L394"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="5"/>
-    <col min="12" max="12" width="8.85546875" style="3"/>
-    <col min="13" max="13" width="8.85546875" style="12"/>
-    <col min="14" max="14" width="8.85546875" style="5"/>
-    <col min="15" max="15" width="8.85546875" style="3"/>
-    <col min="16" max="16" width="8.85546875" style="12"/>
-    <col min="17" max="17" width="8.85546875" style="4"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="5"/>
+    <col min="12" max="12" width="8.83203125" style="3"/>
+    <col min="13" max="13" width="8.83203125" style="12"/>
+    <col min="14" max="14" width="8.83203125" style="5"/>
+    <col min="15" max="15" width="8.83203125" style="3"/>
+    <col min="16" max="16" width="8.83203125" style="12"/>
+    <col min="17" max="17" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -633,7 +633,7 @@
         <v>0.83399999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -659,7 +659,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="2">
-        <v>900.375</v>
+        <v>0.375</v>
       </c>
       <c r="J3" t="s">
         <v>20</v>
@@ -686,7 +686,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -739,7 +739,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -792,7 +792,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -845,7 +845,7 @@
         <v>0.99299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -898,7 +898,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -951,7 +951,7 @@
         <v>0.92400000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>0.94299999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>0.93899999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>0.98399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>0.98699999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>0.96299999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>0.95599999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>0.95099999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>0.97699999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>0.98699999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>0.98899999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>0.95099999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>0.95599999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>0.95599999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>0.96599999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>0.99099999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>0.98399999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>0.91400000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0.90600000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>0.86499999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>0.94699999999999995</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>0.95499999999999996</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>0.96399999999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>0.97199999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>0.91700000000000004</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>0.878</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>1</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>0.878</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>0.91800000000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>0.94699999999999995</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>0.95699999999999996</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>0.94699999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>0.89800000000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>1</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>0.88400000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>0.86499999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>1</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>1</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>0.96199999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>0.97099999999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>1</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>0.93799999999999994</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>1</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>0.98699999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>0.91800000000000004</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>0.93700000000000006</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>1</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>0.90200000000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>0.94899999999999995</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>1</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>0.94599999999999995</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>1</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>1</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>0.84899999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>1</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>1</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>1</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>0.85399999999999998</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>1</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>1</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>0.98899999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>1</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>0.90400000000000003</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>1</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>1</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>0.91800000000000004</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>1</v>
       </c>
@@ -5472,7 +5472,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>0.91369999999999996</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>1</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>0.98899999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>1</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>0.95699999999999996</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>1</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>0.91600000000000004</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>1</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>1</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>0.90600000000000003</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>1</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>1</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>1</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>1</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>1</v>
       </c>
@@ -6037,7 +6037,7 @@
         <v>0.94799999999999995</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>1</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>1</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>0.99399999999999999</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>1</v>
       </c>
@@ -6196,7 +6196,7 @@
         <v>0.98399999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>1</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>1</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>1</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>1</v>
       </c>
@@ -6406,7 +6406,7 @@
         <v>0.90600000000000003</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>1</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>1</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>0.95799999999999996</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>1</v>
       </c>
@@ -6556,7 +6556,7 @@
         <v>0.95599999999999996</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>1</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>0.91800000000000004</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>1</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>1</v>
       </c>
@@ -6715,7 +6715,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>1</v>
       </c>
@@ -6768,7 +6768,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>1</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>0.89700000000000002</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>1</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>0.91900000000000004</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>1</v>
       </c>
@@ -6918,7 +6918,7 @@
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>1</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>1</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>0.94799999999999995</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>1</v>
       </c>
@@ -7077,7 +7077,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>1</v>
       </c>
@@ -7130,7 +7130,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>1</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>0.98699999999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>1</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>1</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>1</v>
       </c>
@@ -7342,7 +7342,7 @@
         <v>0.86599999999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>1</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>0.877</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>1</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>0.92200000000000004</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>1</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>0.95699999999999996</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>1</v>
       </c>
@@ -7545,7 +7545,7 @@
         <v>0.96299999999999997</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>1</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>1</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>1</v>
       </c>
@@ -7704,7 +7704,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>1</v>
       </c>
@@ -7757,7 +7757,7 @@
         <v>0.94299999999999995</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>1</v>
       </c>
@@ -7810,7 +7810,7 @@
         <v>0.92600000000000005</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>1</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>0.92300000000000004</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>1</v>
       </c>
@@ -7916,7 +7916,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>1</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>0.86199999999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>1</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>1</v>
       </c>
@@ -8063,7 +8063,7 @@
         <v>0.93700000000000006</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>1</v>
       </c>
@@ -8116,7 +8116,7 @@
         <v>0.96399999999999997</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>1</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>0.91600000000000004</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>1</v>
       </c>
@@ -8222,7 +8222,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>1</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>1</v>
       </c>
@@ -8328,7 +8328,7 @@
         <v>0.91400000000000003</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>1</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>1</v>
       </c>
@@ -8434,7 +8434,7 @@
         <v>0.92600000000000005</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>1</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>1</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>0.95499999999999996</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>1</v>
       </c>
@@ -8584,7 +8584,7 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>1</v>
       </c>
@@ -8637,7 +8637,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>1</v>
       </c>
@@ -8690,7 +8690,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>1</v>
       </c>
@@ -8743,7 +8743,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>1</v>
       </c>
@@ -8796,7 +8796,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>1</v>
       </c>
@@ -8849,7 +8849,7 @@
         <v>0.88900000000000001</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>1</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>1</v>
       </c>
@@ -8946,7 +8946,7 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>1</v>
       </c>
@@ -8999,7 +8999,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>1</v>
       </c>
@@ -9052,7 +9052,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>1</v>
       </c>
@@ -9105,7 +9105,7 @@
         <v>0.91600000000000004</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>1</v>
       </c>
@@ -9158,7 +9158,7 @@
         <v>0.91900000000000004</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>1</v>
       </c>
@@ -9211,7 +9211,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>1</v>
       </c>
@@ -9264,7 +9264,7 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>1</v>
       </c>
@@ -9317,7 +9317,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>1</v>
       </c>
@@ -9361,7 +9361,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>1</v>
       </c>
@@ -9414,7 +9414,7 @@
         <v>0.95399999999999996</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>1</v>
       </c>
@@ -9465,7 +9465,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>1</v>
       </c>
@@ -9518,7 +9518,7 @@
         <v>0.98399999999999999</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>1</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>0.93400000000000005</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>1</v>
       </c>
@@ -9624,7 +9624,7 @@
         <v>0.92300000000000004</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>1</v>
       </c>
@@ -9677,7 +9677,7 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>1</v>
       </c>
@@ -9730,7 +9730,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>1</v>
       </c>
@@ -9774,7 +9774,7 @@
         <v>0.871</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>1</v>
       </c>
@@ -9827,7 +9827,7 @@
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>1</v>
       </c>
@@ -9880,7 +9880,7 @@
         <v>0.97199999999999998</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>1</v>
       </c>
@@ -9933,7 +9933,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>1</v>
       </c>
@@ -9986,7 +9986,7 @@
         <v>0.90200000000000002</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>1</v>
       </c>
@@ -10039,7 +10039,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>1</v>
       </c>
@@ -10092,7 +10092,7 @@
         <v>0.91400000000000003</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>1</v>
       </c>
@@ -10145,7 +10145,7 @@
         <v>0.90500000000000003</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>1</v>
       </c>
@@ -10189,7 +10189,7 @@
         <v>0.91900000000000004</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>1</v>
       </c>
@@ -10242,7 +10242,7 @@
         <v>0.97299999999999998</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>1</v>
       </c>
@@ -10295,7 +10295,7 @@
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>1</v>
       </c>
@@ -10348,7 +10348,7 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>1</v>
       </c>
@@ -10401,7 +10401,7 @@
         <v>0.91800000000000004</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>1</v>
       </c>
@@ -10454,7 +10454,7 @@
         <v>0.90400000000000003</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>1</v>
       </c>
@@ -10507,7 +10507,7 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>1</v>
       </c>
@@ -10560,7 +10560,7 @@
         <v>0.92400000000000004</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>1</v>
       </c>
@@ -10604,7 +10604,7 @@
         <v>0.878</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>1</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>1</v>
       </c>
@@ -10710,7 +10710,7 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>1</v>
       </c>
@@ -10763,7 +10763,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>1</v>
       </c>
@@ -10816,7 +10816,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>1</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>0.96299999999999997</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>1</v>
       </c>
@@ -10922,7 +10922,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>1</v>
       </c>
@@ -10975,7 +10975,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>1</v>
       </c>
@@ -11028,7 +11028,7 @@
         <v>0.874</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>1</v>
       </c>
@@ -11072,7 +11072,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>1</v>
       </c>
@@ -11125,7 +11125,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>1</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>0.94599999999999995</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>1</v>
       </c>
@@ -11231,7 +11231,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>1</v>
       </c>
@@ -11284,7 +11284,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>1</v>
       </c>
@@ -11337,7 +11337,7 @@
         <v>0.96399999999999997</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>1</v>
       </c>
@@ -11390,7 +11390,7 @@
         <v>0.95899999999999996</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>1</v>
       </c>
@@ -11443,7 +11443,7 @@
         <v>0.92300000000000004</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>1</v>
       </c>
@@ -11496,7 +11496,7 @@
         <v>0.90800000000000003</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>1</v>
       </c>
@@ -11540,7 +11540,7 @@
         <v>0.79800000000000004</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>1</v>
       </c>
@@ -11593,7 +11593,7 @@
         <v>0.92300000000000004</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>1</v>
       </c>
@@ -11646,7 +11646,7 @@
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>1</v>
       </c>
@@ -11699,7 +11699,7 @@
         <v>0.95699999999999996</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>1</v>
       </c>
@@ -11752,7 +11752,7 @@
         <v>0.97399999999999998</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>1</v>
       </c>
@@ -11805,7 +11805,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>1</v>
       </c>
@@ -11858,7 +11858,7 @@
         <v>0.91600000000000004</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>1</v>
       </c>
@@ -11911,7 +11911,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>1</v>
       </c>
@@ -11955,7 +11955,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>1</v>
       </c>
@@ -12008,7 +12008,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>1</v>
       </c>
@@ -12061,7 +12061,7 @@
         <v>0.91400000000000003</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>1</v>
       </c>
@@ -12114,7 +12114,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>1</v>
       </c>
@@ -12167,7 +12167,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>1</v>
       </c>
@@ -12220,7 +12220,7 @@
         <v>0.91700000000000004</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>1</v>
       </c>
@@ -12273,7 +12273,7 @@
         <v>0.92400000000000004</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>1</v>
       </c>
@@ -12326,7 +12326,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>1</v>
       </c>
@@ -12379,7 +12379,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>1</v>
       </c>
@@ -12423,7 +12423,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>1</v>
       </c>
@@ -12476,7 +12476,7 @@
         <v>0.95399999999999996</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>1</v>
       </c>
@@ -12529,7 +12529,7 @@
         <v>0.95499999999999996</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>1</v>
       </c>
@@ -12582,7 +12582,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>1</v>
       </c>
@@ -12635,7 +12635,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>1</v>
       </c>
@@ -12688,7 +12688,7 @@
         <v>0.90400000000000003</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>1</v>
       </c>
@@ -12741,7 +12741,7 @@
         <v>0.88200000000000001</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>1</v>
       </c>
@@ -12794,7 +12794,7 @@
         <v>0.89200000000000002</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>1</v>
       </c>
@@ -12838,7 +12838,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>1</v>
       </c>
@@ -12891,7 +12891,7 @@
         <v>0.95499999999999996</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>1</v>
       </c>
@@ -12944,7 +12944,7 @@
         <v>0.95599999999999996</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>1</v>
       </c>
@@ -12997,7 +12997,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>1</v>
       </c>
@@ -13050,7 +13050,7 @@
         <v>0.89700000000000002</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>1</v>
       </c>
@@ -13103,7 +13103,7 @@
         <v>0.98699999999999999</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>1</v>
       </c>
@@ -13156,7 +13156,7 @@
         <v>0.91100000000000003</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>1</v>
       </c>
@@ -13209,7 +13209,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>1</v>
       </c>
@@ -13262,7 +13262,7 @@
         <v>0.90800000000000003</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>1</v>
       </c>
@@ -13306,7 +13306,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>1</v>
       </c>
@@ -13359,7 +13359,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>1</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>1</v>
       </c>
@@ -13465,7 +13465,7 @@
         <v>0.96199999999999997</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>1</v>
       </c>
@@ -13518,7 +13518,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>1</v>
       </c>
@@ -13571,7 +13571,7 @@
         <v>0.94699999999999995</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>1</v>
       </c>
@@ -13624,7 +13624,7 @@
         <v>0.94499999999999995</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>1</v>
       </c>
@@ -13677,7 +13677,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>1</v>
       </c>
@@ -13722,7 +13722,7 @@
         <v>94.2</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>1</v>
       </c>
@@ -13775,7 +13775,7 @@
         <v>0.97399999999999998</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>1</v>
       </c>
@@ -13828,7 +13828,7 @@
         <v>0.97199999999999998</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>1</v>
       </c>
@@ -13881,7 +13881,7 @@
         <v>0.93400000000000005</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>1</v>
       </c>
@@ -13934,7 +13934,7 @@
         <v>0.93700000000000006</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>1</v>
       </c>
@@ -13987,7 +13987,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>1</v>
       </c>
@@ -14040,7 +14040,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>1</v>
       </c>
@@ -14093,7 +14093,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>1</v>
       </c>
@@ -14137,7 +14137,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>1</v>
       </c>
@@ -14190,7 +14190,7 @@
         <v>0.93700000000000006</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>1</v>
       </c>
@@ -14243,7 +14243,7 @@
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>1</v>
       </c>
@@ -14296,7 +14296,7 @@
         <v>0.95599999999999996</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>1</v>
       </c>
@@ -14349,7 +14349,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>1</v>
       </c>
@@ -14402,7 +14402,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>1</v>
       </c>
@@ -14455,7 +14455,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>1</v>
       </c>
@@ -14508,7 +14508,7 @@
         <v>0.92600000000000005</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>1</v>
       </c>
@@ -14561,7 +14561,7 @@
         <v>0.91400000000000003</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>1</v>
       </c>
@@ -14605,7 +14605,7 @@
         <v>0.96299999999999997</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>1</v>
       </c>
@@ -14658,7 +14658,7 @@
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>1</v>
       </c>
@@ -14711,7 +14711,7 @@
         <v>0.98899999999999999</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>1</v>
       </c>
@@ -14764,7 +14764,7 @@
         <v>0.96599999999999997</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>1</v>
       </c>
@@ -14817,7 +14817,7 @@
         <v>0.93799999999999994</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>1</v>
       </c>
@@ -14870,7 +14870,7 @@
         <v>0.94799999999999995</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>1</v>
       </c>
@@ -14923,7 +14923,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>1</v>
       </c>
@@ -14976,7 +14976,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>1</v>
       </c>
@@ -15020,7 +15020,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>1</v>
       </c>
@@ -15073,7 +15073,7 @@
         <v>0.95799999999999996</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>1</v>
       </c>
@@ -15126,7 +15126,7 @@
         <v>0.94899999999999995</v>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>1</v>
       </c>
@@ -15179,7 +15179,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>1</v>
       </c>
@@ -15232,7 +15232,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>1</v>
       </c>
@@ -15285,7 +15285,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>1</v>
       </c>
@@ -15338,7 +15338,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>1</v>
       </c>
@@ -15391,7 +15391,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>1</v>
       </c>
@@ -15444,7 +15444,7 @@
         <v>0.79600000000000004</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>1</v>
       </c>
@@ -15482,7 +15482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>1</v>
       </c>
@@ -15535,7 +15535,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>1</v>
       </c>
@@ -15588,7 +15588,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>1</v>
       </c>
@@ -15641,7 +15641,7 @@
         <v>0.84799999999999998</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>1</v>
       </c>
@@ -15694,7 +15694,7 @@
         <v>0.83599999999999997</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>1</v>
       </c>
@@ -15747,7 +15747,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>1</v>
       </c>
@@ -15800,7 +15800,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>1</v>
       </c>
@@ -15853,7 +15853,7 @@
         <v>0.82599999999999996</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>1</v>
       </c>
@@ -15897,7 +15897,7 @@
         <v>0.94299999999999995</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>1</v>
       </c>
@@ -15950,7 +15950,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>1</v>
       </c>
@@ -16003,7 +16003,7 @@
         <v>0.97299999999999998</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>1</v>
       </c>
@@ -16056,7 +16056,7 @@
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>1</v>
       </c>
@@ -16109,7 +16109,7 @@
         <v>0.90100000000000002</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>1</v>
       </c>
@@ -16162,7 +16162,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>1</v>
       </c>
@@ -16215,7 +16215,7 @@
         <v>0.94799999999999995</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>1</v>
       </c>
@@ -16268,7 +16268,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>1</v>
       </c>
@@ -16312,7 +16312,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>1</v>
       </c>
@@ -16365,7 +16365,7 @@
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>1</v>
       </c>
@@ -16418,7 +16418,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>1</v>
       </c>
@@ -16471,7 +16471,7 @@
         <v>0.94799999999999995</v>
       </c>
     </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>1</v>
       </c>
@@ -16524,7 +16524,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>1</v>
       </c>
@@ -16577,7 +16577,7 @@
         <v>0.97199999999999998</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>1</v>
       </c>
@@ -16630,7 +16630,7 @@
         <v>0.94699999999999995</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>1</v>
       </c>
@@ -16683,7 +16683,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>1</v>
       </c>
@@ -16736,7 +16736,7 @@
         <v>0.94299999999999995</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>1</v>
       </c>
@@ -16780,7 +16780,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>1</v>
       </c>
@@ -16833,7 +16833,7 @@
         <v>0.94899999999999995</v>
       </c>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>1</v>
       </c>
@@ -16886,7 +16886,7 @@
         <v>0.97099999999999997</v>
       </c>
     </row>
-    <row r="316" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A316" s="7" t="s">
         <v>1</v>
       </c>
@@ -16939,7 +16939,7 @@
         <v>0.96199999999999997</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>1</v>
       </c>
@@ -16992,7 +16992,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>1</v>
       </c>
@@ -17045,7 +17045,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>1</v>
       </c>
@@ -17098,7 +17098,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>1</v>
       </c>
@@ -17151,7 +17151,7 @@
         <v>0.91800000000000004</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>1</v>
       </c>
@@ -17204,7 +17204,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>1</v>
       </c>
@@ -17251,7 +17251,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>1</v>
       </c>
@@ -17304,7 +17304,7 @@
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>1</v>
       </c>
@@ -17357,7 +17357,7 @@
         <v>0.95199999999999996</v>
       </c>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>1</v>
       </c>
@@ -17410,7 +17410,7 @@
         <v>0.93899999999999995</v>
       </c>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>1</v>
       </c>
@@ -17463,7 +17463,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>1</v>
       </c>
@@ -17516,7 +17516,7 @@
         <v>0.89700000000000002</v>
       </c>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>1</v>
       </c>
@@ -17569,7 +17569,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>1</v>
       </c>
@@ -17622,7 +17622,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>1</v>
       </c>
@@ -17660,7 +17660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>1</v>
       </c>
@@ -17713,7 +17713,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>1</v>
       </c>
@@ -17766,7 +17766,7 @@
         <v>0.95199999999999996</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>1</v>
       </c>
@@ -17819,7 +17819,7 @@
         <v>0.91900000000000004</v>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>1</v>
       </c>
@@ -17872,7 +17872,7 @@
         <v>0.89200000000000002</v>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>1</v>
       </c>
@@ -17925,7 +17925,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A336" s="9" t="s">
         <v>1</v>
       </c>
@@ -17978,7 +17978,7 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>1</v>
       </c>
@@ -18031,7 +18031,7 @@
         <v>0.90100000000000002</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A338" s="9" t="s">
         <v>1</v>
       </c>
@@ -18084,7 +18084,7 @@
         <v>0.88400000000000001</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A339" s="9" t="s">
         <v>1</v>
       </c>
@@ -18128,7 +18128,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A340" s="9" t="s">
         <v>1</v>
       </c>
@@ -18178,7 +18178,7 @@
         <v>0.99299999999999999</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A341" s="9" t="s">
         <v>1</v>
       </c>
@@ -18231,7 +18231,7 @@
         <v>0.97199999999999998</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A342" s="9" t="s">
         <v>1</v>
       </c>
@@ -18284,7 +18284,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A343" s="9" t="s">
         <v>1</v>
       </c>
@@ -18337,7 +18337,7 @@
         <v>0.88700000000000001</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A344" s="9" t="s">
         <v>1</v>
       </c>
@@ -18390,7 +18390,7 @@
         <v>0.90400000000000003</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A345" s="9" t="s">
         <v>1</v>
       </c>
@@ -18443,7 +18443,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A346" s="9" t="s">
         <v>1</v>
       </c>
@@ -18496,7 +18496,7 @@
         <v>0.90100000000000002</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A347" s="9" t="s">
         <v>1</v>
       </c>
@@ -18540,7 +18540,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A348" s="9" t="s">
         <v>1</v>
       </c>
@@ -18593,7 +18593,7 @@
         <v>0.97399999999999998</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A349" s="9" t="s">
         <v>1</v>
       </c>
@@ -18646,7 +18646,7 @@
         <v>0.96199999999999997</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A350" s="9" t="s">
         <v>1</v>
       </c>
@@ -18696,7 +18696,7 @@
         <v>0.91700000000000004</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A351" s="9" t="s">
         <v>1</v>
       </c>
@@ -18746,7 +18746,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A352" s="9" t="s">
         <v>1</v>
       </c>
@@ -18799,7 +18799,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A353" s="9" t="s">
         <v>1</v>
       </c>
@@ -18852,7 +18852,7 @@
         <v>0.90800000000000003</v>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A354" s="9" t="s">
         <v>1</v>
       </c>
@@ -18905,7 +18905,7 @@
         <v>0.88900000000000001</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A355" s="9" t="s">
         <v>1</v>
       </c>
@@ -18949,7 +18949,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A356" s="9" t="s">
         <v>1</v>
       </c>
@@ -19002,7 +19002,7 @@
         <v>0.96899999999999997</v>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A357" s="9" t="s">
         <v>1</v>
       </c>
@@ -19055,7 +19055,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A358" s="9" t="s">
         <v>1</v>
       </c>
@@ -19108,7 +19108,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A359" s="9" t="s">
         <v>1</v>
       </c>
@@ -19161,7 +19161,7 @@
         <v>0.91700000000000004</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A360" s="9" t="s">
         <v>1</v>
       </c>
@@ -19211,7 +19211,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A361" s="9" t="s">
         <v>1</v>
       </c>
@@ -19264,7 +19264,7 @@
         <v>0.92600000000000005</v>
       </c>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A362" s="9" t="s">
         <v>1</v>
       </c>
@@ -19317,7 +19317,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A363" s="9" t="s">
         <v>1</v>
       </c>
@@ -19370,7 +19370,7 @@
         <v>0.86599999999999999</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A364" s="9" t="s">
         <v>1</v>
       </c>
@@ -19408,7 +19408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A365" s="9" t="s">
         <v>1</v>
       </c>
@@ -19461,7 +19461,7 @@
         <v>0.95699999999999996</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A366" s="9" t="s">
         <v>1</v>
       </c>
@@ -19514,7 +19514,7 @@
         <v>0.93799999999999994</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A367" s="9" t="s">
         <v>1</v>
       </c>
@@ -19561,7 +19561,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A368" s="9" t="s">
         <v>1</v>
       </c>
@@ -19614,7 +19614,7 @@
         <v>0.88400000000000001</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A369" s="9" t="s">
         <v>1</v>
       </c>
@@ -19667,7 +19667,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A370" s="9" t="s">
         <v>1</v>
       </c>
@@ -19720,7 +19720,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A371" s="9" t="s">
         <v>1</v>
       </c>
@@ -19773,7 +19773,7 @@
         <v>0.872</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A372" s="9" t="s">
         <v>1</v>
       </c>
@@ -19826,7 +19826,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A373" s="9" t="s">
         <v>1</v>
       </c>
@@ -19870,7 +19870,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A374" s="9" t="s">
         <v>1</v>
       </c>
@@ -19923,7 +19923,7 @@
         <v>0.96899999999999997</v>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A375" s="9" t="s">
         <v>1</v>
       </c>
@@ -19976,7 +19976,7 @@
         <v>0.95399999999999996</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A376" s="9" t="s">
         <v>1</v>
       </c>
@@ -20026,7 +20026,7 @@
         <v>0.91700000000000004</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A377" s="9" t="s">
         <v>1</v>
       </c>
@@ -20079,7 +20079,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A378" s="9" t="s">
         <v>1</v>
       </c>
@@ -20132,7 +20132,7 @@
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A379" s="9" t="s">
         <v>1</v>
       </c>
@@ -20185,7 +20185,7 @@
         <v>0.92300000000000004</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A380" s="9" t="s">
         <v>1</v>
       </c>
@@ -20238,7 +20238,7 @@
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A381" s="9" t="s">
         <v>1</v>
       </c>
@@ -20276,7 +20276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A382" s="9" t="s">
         <v>1</v>
       </c>
@@ -20329,7 +20329,7 @@
         <v>0.90400000000000003</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A383" s="9" t="s">
         <v>1</v>
       </c>
@@ -20379,7 +20379,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A384" s="9" t="s">
         <v>1</v>
       </c>
@@ -20432,7 +20432,7 @@
         <v>0.96199999999999997</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A385" s="9" t="s">
         <v>1</v>
       </c>
@@ -20485,7 +20485,7 @@
         <v>0.91600000000000004</v>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A386" s="9" t="s">
         <v>1</v>
       </c>
@@ -20538,7 +20538,7 @@
         <v>0.89700000000000002</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A387" s="9" t="s">
         <v>1</v>
       </c>
@@ -20591,7 +20591,7 @@
         <v>0.88200000000000001</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A388" s="9" t="s">
         <v>1</v>
       </c>
@@ -20644,7 +20644,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A389" s="9" t="s">
         <v>1</v>
       </c>
@@ -20697,7 +20697,7 @@
         <v>0.86199999999999999</v>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A390" s="9" t="s">
         <v>1</v>
       </c>
@@ -20750,7 +20750,7 @@
         <v>0.85099999999999998</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A391" s="9" t="s">
         <v>1</v>
       </c>
@@ -20794,7 +20794,7 @@
         <v>0.77800000000000002</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A392" s="9" t="s">
         <v>1</v>
       </c>
@@ -20847,7 +20847,7 @@
         <v>0.95199999999999996</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A393" s="9" t="s">
         <v>1</v>
       </c>
@@ -20900,7 +20900,7 @@
         <v>0.91700000000000004</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A394" s="9" t="s">
         <v>1</v>
       </c>
@@ -20953,7 +20953,7 @@
         <v>0.89200000000000002</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A395" s="9" t="s">
         <v>1</v>
       </c>
@@ -21006,7 +21006,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A396" s="9" t="s">
         <v>1</v>
       </c>
@@ -21059,7 +21059,7 @@
         <v>0.90800000000000003</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A397" s="9" t="s">
         <v>1</v>
       </c>
@@ -21112,7 +21112,7 @@
         <v>0.89400000000000002</v>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A398" s="9" t="s">
         <v>1</v>
       </c>
@@ -21165,7 +21165,7 @@
         <v>0.95399999999999996</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A399" s="9" t="s">
         <v>1</v>
       </c>
@@ -21218,7 +21218,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A400" s="9" t="s">
         <v>1</v>
       </c>
@@ -21253,7 +21253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A401" s="9" t="s">
         <v>1</v>
       </c>
@@ -21306,7 +21306,7 @@
         <v>0.89800000000000002</v>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A402" s="9" t="s">
         <v>1</v>
       </c>
@@ -21359,7 +21359,7 @@
         <v>0.95399999999999996</v>
       </c>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A403" s="9" t="s">
         <v>1</v>
       </c>
@@ -21409,7 +21409,7 @@
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A404" s="9" t="s">
         <v>1</v>
       </c>
@@ -21462,7 +21462,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A405" s="9" t="s">
         <v>1</v>
       </c>
@@ -21515,7 +21515,7 @@
         <v>0.85099999999999998</v>
       </c>
     </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A406" s="9" t="s">
         <v>1</v>
       </c>
@@ -21568,7 +21568,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A407" s="9" t="s">
         <v>1</v>
       </c>
@@ -21621,7 +21621,7 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A408" s="9" t="s">
         <v>1</v>
       </c>
@@ -21674,7 +21674,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="409" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A409" s="9" t="s">
         <v>1</v>
       </c>

</xml_diff>